<commit_message>
Add Excel import functionality for student data and enhance data display
</commit_message>
<xml_diff>
--- a/assets/format_data_siswa.xlsx
+++ b/assets/format_data_siswa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5b5e5968ba41335/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\absensi_sekolah\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{DF4C92A6-A589-4EDE-BD89-B529ECC33179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA69EEF1-7DD0-434D-938B-303D9D200777}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8635D9F-2A44-49C9-A1AF-42DD4FD808C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
   </bookViews>
@@ -35,23 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Laki-Laki</t>
   </si>
   <si>
-    <t>$2y$10$x7xWgiXMLwF/Rq4oH6Lpz.Jt1jzM5a.q8jUamJ.K4qbyXkgtdoELi</t>
-  </si>
-  <si>
-    <t>guru</t>
-  </si>
-  <si>
-    <t>nama_guru</t>
-  </si>
-  <si>
-    <t>nip</t>
-  </si>
-  <si>
     <t>jenis_kelamin</t>
   </si>
   <si>
@@ -61,37 +49,52 @@
     <t>alamat</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
     <t>mjl</t>
   </si>
   <si>
-    <t>Guru_A</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Guru_B</t>
-  </si>
-  <si>
-    <t>Guru_C</t>
-  </si>
-  <si>
-    <t>Guru_D</t>
-  </si>
-  <si>
-    <t>Guru_E</t>
-  </si>
-  <si>
-    <t>Guru_F</t>
-  </si>
-  <si>
-    <t>Guru_G</t>
+    <t>nisn</t>
+  </si>
+  <si>
+    <t>nama_siswa</t>
+  </si>
+  <si>
+    <t>id_kelas</t>
+  </si>
+  <si>
+    <t>nis</t>
+  </si>
+  <si>
+    <t>Siswa1</t>
+  </si>
+  <si>
+    <t>Siswa2</t>
+  </si>
+  <si>
+    <t>Siswa3</t>
+  </si>
+  <si>
+    <t>Siswa4</t>
+  </si>
+  <si>
+    <t>Siswa5</t>
+  </si>
+  <si>
+    <t>Siswa6</t>
+  </si>
+  <si>
+    <t>Siswa7</t>
+  </si>
+  <si>
+    <t>Siswa8</t>
+  </si>
+  <si>
+    <t>Siswa9</t>
+  </si>
+  <si>
+    <t>Siswa10</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
   </si>
 </sst>
 </file>
@@ -462,205 +465,270 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>26549414</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>12345678</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>37147</v>
+        <v>36974</v>
       </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>26549415</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>12345678</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>37148</v>
+        <v>36975</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2345679</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>12345679</v>
+      <c r="A4" s="1">
+        <v>26549416</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>37149</v>
+        <v>36976</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2345680</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>12345680</v>
+      <c r="A5" s="1">
+        <v>26549417</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>37150</v>
+        <v>36977</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2345681</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>12345681</v>
+      <c r="A6" s="1">
+        <v>26549418</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>37151</v>
+        <v>36978</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2345682</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="1">
+        <v>26549419</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2">
+        <v>36979</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2345683</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>26549420</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>36980</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2345684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>26549421</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>36981</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2345685</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>26549422</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>12345682</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>37152</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2">
+        <v>36982</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2345686</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>26549423</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>12345683</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>37153</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <v>36983</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2345687</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>

</xml_diff>

<commit_message>
Update student import functionality to include NIS and adjust data handling
</commit_message>
<xml_diff>
--- a/assets/format_data_siswa.xlsx
+++ b/assets/format_data_siswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\absensi_sekolah\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8635D9F-2A44-49C9-A1AF-42DD4FD808C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C85715A-6658-4BEB-A6D1-3C4CDB947DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
+    <workbookView xWindow="1200" yWindow="768" windowWidth="17280" windowHeight="9072" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,7 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>2345680</v>
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>2345681</v>
@@ -609,7 +609,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>2345682</v>

</xml_diff>